<commit_message>
Documentation and st changes
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
@@ -727,9 +727,6 @@
     <t>Passes the new buff name and whether it was gained or lost.</t>
   </si>
   <si>
-    <t>Passes the old and new status. The syntax here needs to change.</t>
-  </si>
-  <si>
     <t>Passes any self commands, which are triggered by //gs c &lt;command&gt;</t>
   </si>
   <si>
@@ -769,7 +766,10 @@
     <t>Reloads the current lua document</t>
   </si>
   <si>
-    <t>status_change(new,{type='Status Change',old=old})</t>
+    <t>status_change(new,old)</t>
+  </si>
+  <si>
+    <t>Passes the new and old status.</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C98" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1354,7 @@
         <v>82</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
         <v>90</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
         <v>95</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
@@ -2228,10 +2228,10 @@
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="10"/>
       <c r="E105" t="s">
+        <v>245</v>
+      </c>
+      <c r="G105" t="s">
         <v>246</v>
-      </c>
-      <c r="G105" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
@@ -2249,7 +2249,7 @@
         <v>229</v>
       </c>
       <c r="G107" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="110" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2441,48 +2441,48 @@
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E129" t="s">
         <v>234</v>
       </c>
-      <c r="E129" t="s">
+      <c r="G129" t="s">
         <v>235</v>
-      </c>
-      <c r="G129" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="8"/>
       <c r="E130" t="s">
+        <v>236</v>
+      </c>
+      <c r="G130" t="s">
         <v>237</v>
-      </c>
-      <c r="G130" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" s="8"/>
       <c r="E131" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="8"/>
       <c r="E132" t="s">
+        <v>239</v>
+      </c>
+      <c r="G132" t="s">
         <v>240</v>
-      </c>
-      <c r="G132" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E133" t="s">
+        <v>243</v>
+      </c>
+      <c r="G133" t="s">
         <v>244</v>
-      </c>
-      <c r="G133" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gearswap 0.605 and register_event for SC/BM
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="261">
   <si>
     <t>Old Variable Name</t>
   </si>
@@ -468,15 +468,6 @@
     <t>command</t>
   </si>
   <si>
-    <t>send_command()</t>
-  </si>
-  <si>
-    <t>register_event()</t>
-  </si>
-  <si>
-    <t>write()</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -601,9 +592,6 @@
   </si>
   <si>
     <t>Delays the current spell by however many seconds you choose.</t>
-  </si>
-  <si>
-    <t>Sends a command to console. Be aware that this will (probably?) be picked up by Shortcuts and thus may be picked up again by Gearswap. Don't make an infinite loop.</t>
   </si>
   <si>
     <r>
@@ -634,9 +622,6 @@
     <t>Forces the command to be sent out. Can be used in combination with verify_equip() if you desire.</t>
   </si>
   <si>
-    <t>Allows users to register events in Lua that will be called by LuaCore directly. See the doku wiki for more details about options here. I'd call this "Advanced Mode."</t>
-  </si>
-  <si>
     <t>Writes directly to console.</t>
   </si>
   <si>
@@ -800,6 +785,33 @@
   </si>
   <si>
     <t>Pulled from the player array. Uses "MON" as the code for monipulator. Value determines which Lua file is loaded.</t>
+  </si>
+  <si>
+    <t>disable(slot1,slot2,...)</t>
+  </si>
+  <si>
+    <t>enable(slot1,slot2,...)</t>
+  </si>
+  <si>
+    <t>Disables gear swaps in a given slot.</t>
+  </si>
+  <si>
+    <t>Enables gear swaps in a given slot (reverses disable).</t>
+  </si>
+  <si>
+    <t>send_command(command)</t>
+  </si>
+  <si>
+    <t>write(phrase_to_write)</t>
+  </si>
+  <si>
+    <t>Sends a command to console. Be aware that this will (probably?) be picked up by Shortcuts and thus may be picked up again by Gearswap. Don't make an infinite loop. Also, forces the command to be prefixed by @.</t>
+  </si>
+  <si>
+    <t>windower.register_event()</t>
+  </si>
+  <si>
+    <t>Allows users to register events in Lua that will be called by LuaCore directly. See the doku wiki for more details about options here. I'd call this "Super Advanced Mode."</t>
   </si>
 </sst>
 </file>
@@ -1191,23 +1203,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G137"/>
+  <dimension ref="B1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="124.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="124.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="25.95" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:7" ht="25.9" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1217,10 +1229,10 @@
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C2" s="9" t="s">
         <v>143</v>
       </c>
@@ -1229,7 +1241,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
@@ -1240,10 +1252,10 @@
         <v>141</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>4</v>
@@ -1252,10 +1264,10 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" t="s">
         <v>6</v>
@@ -1264,10 +1276,10 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>8</v>
@@ -1276,10 +1288,10 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" t="s">
         <v>10</v>
@@ -1288,10 +1300,10 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" t="s">
         <v>12</v>
@@ -1300,10 +1312,10 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" t="s">
         <v>14</v>
@@ -1312,10 +1324,10 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" t="s">
         <v>16</v>
@@ -1324,10 +1336,10 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" t="s">
         <v>18</v>
@@ -1336,10 +1348,10 @@
         <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>20</v>
@@ -1348,10 +1360,10 @@
         <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" t="s">
         <v>77</v>
@@ -1360,10 +1372,10 @@
         <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" t="s">
         <v>79</v>
@@ -1372,10 +1384,10 @@
         <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" t="s">
         <v>81</v>
@@ -1384,10 +1396,10 @@
         <v>82</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>83</v>
@@ -1396,10 +1408,10 @@
         <v>84</v>
       </c>
       <c r="G17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>85</v>
@@ -1408,10 +1420,10 @@
         <v>86</v>
       </c>
       <c r="G18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" t="s">
         <v>87</v>
@@ -1420,10 +1432,10 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
@@ -1434,10 +1446,10 @@
         <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" t="s">
         <v>26</v>
@@ -1446,10 +1458,10 @@
         <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" t="s">
         <v>31</v>
@@ -1458,10 +1470,10 @@
         <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" t="s">
         <v>33</v>
@@ -1470,10 +1482,10 @@
         <v>34</v>
       </c>
       <c r="G25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" t="s">
         <v>35</v>
@@ -1482,10 +1494,10 @@
         <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" t="s">
         <v>37</v>
@@ -1494,10 +1506,10 @@
         <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" t="s">
         <v>38</v>
@@ -1506,10 +1518,10 @@
         <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" t="s">
         <v>41</v>
@@ -1518,10 +1530,10 @@
         <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" t="s">
         <v>43</v>
@@ -1530,10 +1542,10 @@
         <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" t="s">
         <v>45</v>
@@ -1542,10 +1554,10 @@
         <v>49</v>
       </c>
       <c r="G31" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" t="s">
         <v>46</v>
@@ -1554,10 +1566,10 @@
         <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" t="s">
         <v>47</v>
@@ -1566,10 +1578,10 @@
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" t="s">
         <v>48</v>
@@ -1578,10 +1590,10 @@
         <v>52</v>
       </c>
       <c r="G34" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" t="s">
         <v>54</v>
@@ -1590,10 +1602,10 @@
         <v>55</v>
       </c>
       <c r="G35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" t="s">
         <v>56</v>
@@ -1602,10 +1614,10 @@
         <v>57</v>
       </c>
       <c r="G36" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" t="s">
         <v>72</v>
@@ -1614,10 +1626,10 @@
         <v>89</v>
       </c>
       <c r="G37" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" t="s">
         <v>73</v>
@@ -1626,10 +1638,10 @@
         <v>90</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" t="s">
         <v>74</v>
@@ -1638,10 +1650,10 @@
         <v>91</v>
       </c>
       <c r="G39" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" t="s">
         <v>75</v>
@@ -1650,10 +1662,10 @@
         <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" t="s">
         <v>76</v>
@@ -1662,28 +1674,28 @@
         <v>93</v>
       </c>
       <c r="G41" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="E42" t="s">
         <v>94</v>
       </c>
       <c r="G42" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="E43" t="s">
         <v>95</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" t="s">
         <v>2</v>
@@ -1692,28 +1704,28 @@
         <v>96</v>
       </c>
       <c r="G44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="E45" t="s">
         <v>97</v>
       </c>
       <c r="G45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="E46" t="s">
         <v>98</v>
       </c>
       <c r="G46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" t="s">
         <v>99</v>
@@ -1722,10 +1734,10 @@
         <v>120</v>
       </c>
       <c r="G47" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" t="s">
         <v>100</v>
@@ -1734,10 +1746,10 @@
         <v>121</v>
       </c>
       <c r="G48" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" t="s">
         <v>101</v>
@@ -1746,10 +1758,10 @@
         <v>122</v>
       </c>
       <c r="G49" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" t="s">
         <v>102</v>
@@ -1758,16 +1770,16 @@
         <v>123</v>
       </c>
       <c r="G50" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="8"/>
       <c r="C51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>104</v>
       </c>
@@ -1778,10 +1790,10 @@
         <v>106</v>
       </c>
       <c r="G55" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="8"/>
       <c r="C56" t="s">
         <v>107</v>
@@ -1790,10 +1802,10 @@
         <v>108</v>
       </c>
       <c r="G56" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
       <c r="C57" t="s">
         <v>109</v>
@@ -1802,10 +1814,10 @@
         <v>110</v>
       </c>
       <c r="G57" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" t="s">
         <v>111</v>
@@ -1814,10 +1826,10 @@
         <v>112</v>
       </c>
       <c r="G58" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
       <c r="C59" t="s">
         <v>115</v>
@@ -1826,10 +1838,10 @@
         <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
       <c r="C60" t="s">
         <v>113</v>
@@ -1838,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="8" t="s">
         <v>116</v>
       </c>
@@ -1852,10 +1864,10 @@
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" t="s">
         <v>118</v>
@@ -1864,10 +1876,10 @@
         <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
       <c r="C65" t="s">
         <v>119</v>
@@ -1876,10 +1888,10 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>29</v>
       </c>
@@ -1890,10 +1902,10 @@
         <v>30</v>
       </c>
       <c r="G68" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="8"/>
       <c r="C69" t="s">
         <v>58</v>
@@ -1902,10 +1914,10 @@
         <v>59</v>
       </c>
       <c r="G69" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" t="s">
         <v>60</v>
@@ -1914,10 +1926,10 @@
         <v>61</v>
       </c>
       <c r="G70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="8"/>
       <c r="C71" t="s">
         <v>63</v>
@@ -1926,10 +1938,10 @@
         <v>62</v>
       </c>
       <c r="G71" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="8"/>
       <c r="C72" t="s">
         <v>64</v>
@@ -1938,10 +1950,10 @@
         <v>65</v>
       </c>
       <c r="G72" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" t="s">
         <v>66</v>
@@ -1950,10 +1962,10 @@
         <v>67</v>
       </c>
       <c r="G73" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" t="s">
         <v>68</v>
@@ -1962,10 +1974,10 @@
         <v>70</v>
       </c>
       <c r="G74" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
       <c r="C75" t="s">
         <v>69</v>
@@ -1974,60 +1986,60 @@
         <v>71</v>
       </c>
       <c r="G75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C78" t="s">
         <v>53</v>
       </c>
       <c r="E78" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G78" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="8"/>
       <c r="C79" t="s">
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G79" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" t="s">
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G80" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
       <c r="C81" t="s">
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G81" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" ht="21" x14ac:dyDescent="0.4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B83" s="4" t="s">
         <v>128</v>
       </c>
@@ -2038,10 +2050,10 @@
         <v>129</v>
       </c>
       <c r="G83" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>127</v>
       </c>
@@ -2052,34 +2064,34 @@
         <v>144</v>
       </c>
       <c r="G86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="8"/>
       <c r="C87" t="s">
         <v>132</v>
       </c>
       <c r="E87" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G87" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
       <c r="C88" t="s">
         <v>139</v>
       </c>
       <c r="E88" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G88" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
       <c r="C89" t="s">
         <v>140</v>
@@ -2088,34 +2100,34 @@
         <v>142</v>
       </c>
       <c r="G89" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
       <c r="C90" t="s">
         <v>125</v>
       </c>
       <c r="E90" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G90" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="8"/>
       <c r="C91" t="s">
         <v>149</v>
       </c>
       <c r="E91" t="s">
-        <v>150</v>
+        <v>256</v>
       </c>
       <c r="G91" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="8"/>
       <c r="C92" t="s">
         <v>2</v>
@@ -2124,10 +2136,10 @@
         <v>138</v>
       </c>
       <c r="G92" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="8"/>
       <c r="C93" t="s">
         <v>2</v>
@@ -2136,10 +2148,10 @@
         <v>148</v>
       </c>
       <c r="G93" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="8"/>
       <c r="C94" t="s">
         <v>2</v>
@@ -2148,10 +2160,10 @@
         <v>145</v>
       </c>
       <c r="G94" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="8"/>
       <c r="C95" t="s">
         <v>2</v>
@@ -2160,10 +2172,10 @@
         <v>146</v>
       </c>
       <c r="G95" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="8"/>
       <c r="C96" t="s">
         <v>2</v>
@@ -2172,46 +2184,46 @@
         <v>147</v>
       </c>
       <c r="G96" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="8"/>
       <c r="C97" t="s">
         <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>151</v>
+        <v>259</v>
       </c>
       <c r="G97" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="8"/>
       <c r="C98" t="s">
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>152</v>
+        <v>257</v>
       </c>
       <c r="G98" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="8"/>
       <c r="C99" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E99" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G99" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="8"/>
       <c r="C100" t="s">
         <v>130</v>
@@ -2220,360 +2232,384 @@
         <v>2</v>
       </c>
       <c r="G100" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="8"/>
+      <c r="C101" t="s">
+        <v>133</v>
+      </c>
+      <c r="E101" t="s">
+        <v>252</v>
+      </c>
+      <c r="G101" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
+      <c r="C102" t="s">
+        <v>134</v>
+      </c>
+      <c r="E102" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="101" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B102" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="E102" t="s">
-        <v>246</v>
-      </c>
       <c r="G102" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="10"/>
-      <c r="C103" t="s">
-        <v>216</v>
-      </c>
-      <c r="E103" t="s">
-        <v>224</v>
-      </c>
-      <c r="G103" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="10"/>
-      <c r="C104" t="s">
-        <v>217</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="2"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="10" t="s">
+        <v>220</v>
       </c>
       <c r="E104" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="G104" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="10"/>
       <c r="C105" t="s">
+        <v>211</v>
+      </c>
+      <c r="E105" t="s">
+        <v>219</v>
+      </c>
+      <c r="G105" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="10"/>
+      <c r="C106" t="s">
+        <v>212</v>
+      </c>
+      <c r="E106" t="s">
         <v>218</v>
       </c>
-      <c r="E105" t="s">
+      <c r="G106" t="s">
         <v>222</v>
       </c>
-      <c r="G105" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="10"/>
-      <c r="E106" t="s">
-        <v>221</v>
-      </c>
-      <c r="G106" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="10"/>
+      <c r="C107" t="s">
+        <v>213</v>
+      </c>
       <c r="E107" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G107" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="10"/>
       <c r="E108" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="G108" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="10"/>
       <c r="E109" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G109" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="10"/>
       <c r="E110" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="G110" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="10"/>
       <c r="E111" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="G111" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="10"/>
+      <c r="E112" t="s">
+        <v>221</v>
+      </c>
+      <c r="G112" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="10"/>
+      <c r="E113" t="s">
+        <v>239</v>
+      </c>
+      <c r="G113" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C116" t="s">
         <v>135</v>
       </c>
-      <c r="E114" t="s">
-        <v>2</v>
-      </c>
-      <c r="G114" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="8"/>
-      <c r="C115" t="s">
-        <v>124</v>
-      </c>
-      <c r="E115" t="s">
-        <v>2</v>
-      </c>
-      <c r="G115" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="8"/>
-      <c r="C116" t="s">
-        <v>126</v>
-      </c>
       <c r="E116" t="s">
         <v>2</v>
       </c>
       <c r="G116" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="8"/>
       <c r="C117" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E117" t="s">
         <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="8"/>
       <c r="C118" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E118" t="s">
         <v>2</v>
       </c>
       <c r="G118" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="8"/>
       <c r="C119" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E119" t="s">
         <v>2</v>
       </c>
       <c r="G119" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="8"/>
       <c r="C120" t="s">
+        <v>134</v>
+      </c>
+      <c r="E120" t="s">
+        <v>2</v>
+      </c>
+      <c r="G120" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="8"/>
+      <c r="C121" t="s">
+        <v>137</v>
+      </c>
+      <c r="E121" t="s">
+        <v>2</v>
+      </c>
+      <c r="G121" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="8"/>
+      <c r="C122" t="s">
         <v>130</v>
       </c>
-      <c r="E120" t="s">
-        <v>2</v>
-      </c>
-      <c r="G120" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="3"/>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B123" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C123" t="s">
-        <v>2</v>
-      </c>
-      <c r="E123" t="s">
-        <v>153</v>
-      </c>
-      <c r="G123" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B124" s="10"/>
-      <c r="C124" t="s">
-        <v>2</v>
-      </c>
-      <c r="E124" t="s">
+      <c r="E122" t="s">
+        <v>2</v>
+      </c>
+      <c r="G122" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="3"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="G124" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B125" s="10"/>
       <c r="C125" t="s">
         <v>2</v>
       </c>
       <c r="E125" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G125" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="10"/>
       <c r="C126" t="s">
         <v>2</v>
       </c>
       <c r="E126" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G126" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="10"/>
       <c r="C127" t="s">
         <v>2</v>
       </c>
       <c r="E127" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G127" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128" s="10"/>
       <c r="C128" t="s">
         <v>2</v>
       </c>
       <c r="E128" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G128" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="10"/>
       <c r="C129" t="s">
         <v>2</v>
       </c>
       <c r="E129" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G129" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="10"/>
       <c r="C130" t="s">
         <v>2</v>
       </c>
       <c r="E130" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G130" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B133" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E133" t="s">
-        <v>231</v>
-      </c>
-      <c r="G133" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B134" s="8"/>
-      <c r="E134" t="s">
-        <v>233</v>
-      </c>
-      <c r="G134" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B135" s="8"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="10"/>
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+      <c r="E131" t="s">
+        <v>157</v>
+      </c>
+      <c r="G131" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="10"/>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+      <c r="E132" t="s">
+        <v>158</v>
+      </c>
+      <c r="G132" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="8" t="s">
+        <v>225</v>
+      </c>
       <c r="E135" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="G135" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
       <c r="E136" t="s">
+        <v>228</v>
+      </c>
+      <c r="G136" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="8"/>
+      <c r="E137" t="s">
+        <v>230</v>
+      </c>
+      <c r="G137" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B138" s="8"/>
+      <c r="E138" t="s">
+        <v>231</v>
+      </c>
+      <c r="G138" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E139" t="s">
+        <v>235</v>
+      </c>
+      <c r="G139" t="s">
         <v>236</v>
-      </c>
-      <c r="G136" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E137" t="s">
-        <v>240</v>
-      </c>
-      <c r="G137" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B133:B136"/>
+    <mergeCell ref="B135:B138"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="B123:B130"/>
+    <mergeCell ref="B125:B132"/>
     <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B114:B120"/>
+    <mergeCell ref="B116:B122"/>
     <mergeCell ref="B22:B51"/>
     <mergeCell ref="B4:B19"/>
     <mergeCell ref="B55:B60"/>
     <mergeCell ref="B63:B65"/>
     <mergeCell ref="B68:B75"/>
-    <mergeCell ref="B102:B111"/>
-    <mergeCell ref="B86:B100"/>
+    <mergeCell ref="B104:B113"/>
+    <mergeCell ref="B86:B102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2586,7 +2622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2598,7 +2634,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Gearswap v0.705 - Fixed line 71 and 324 errors
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="269">
   <si>
     <t>Old Variable Name</t>
   </si>
@@ -824,6 +824,18 @@
   </si>
   <si>
     <t>This will run the file at ../gearswap/data/file_name.lua and add all values returned from it in a table to the user environment.</t>
+  </si>
+  <si>
+    <t>//gs disable &lt;optional slot&gt;</t>
+  </si>
+  <si>
+    <t>//gs enable &lt;optional slot&gt;</t>
+  </si>
+  <si>
+    <t>Disables equip commands targeting a given slot. "All" will prevent all equip commands. Providing no second argument will disable user gearswap file execution, although registered events will still run.</t>
+  </si>
+  <si>
+    <t>Enables equip commands targeting a given slot. "All" will allow all equip commands. Providing no second argument will enable user gearswap file execution, although registered events will still run.</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G140"/>
+  <dimension ref="B1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,7 +2577,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="8" t="s">
         <v>225</v>
       </c>
@@ -2576,7 +2588,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
       <c r="E136" t="s">
         <v>228</v>
@@ -2585,7 +2597,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="8"/>
       <c r="E137" t="s">
         <v>230</v>
@@ -2594,7 +2606,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="8"/>
       <c r="E138" t="s">
         <v>231</v>
@@ -2603,7 +2615,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="139" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="8"/>
       <c r="E139" t="s">
         <v>235</v>
       </c>
@@ -2611,7 +2624,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="8"/>
       <c r="C140" t="s">
         <v>259</v>
       </c>
@@ -2622,9 +2636,26 @@
         <v>261</v>
       </c>
     </row>
+    <row r="141" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="8"/>
+      <c r="E141" t="s">
+        <v>266</v>
+      </c>
+      <c r="G141" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="8"/>
+      <c r="E142" t="s">
+        <v>265</v>
+      </c>
+      <c r="G142" t="s">
+        <v>267</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B135:B138"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="B125:B132"/>
     <mergeCell ref="B78:B81"/>
@@ -2636,6 +2667,7 @@
     <mergeCell ref="B68:B75"/>
     <mergeCell ref="B104:B113"/>
     <mergeCell ref="B86:B102"/>
+    <mergeCell ref="B135:B142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Gearswap v0.706 - Export Sets
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -814,9 +814,6 @@
     <t>//gs export &lt;options&gt;</t>
   </si>
   <si>
-    <t>Exports your currently equipped gear or inventory into gearswap .lua or spellcast .xml format. Takes options "inventory" and "xml." Defaults to currently equipped gear and lua otherwise.</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -836,6 +833,9 @@
   </si>
   <si>
     <t>Enables equip commands targeting a given slot. "All" will allow all equip commands. Providing no second argument will enable user gearswap file execution, although registered events will still run.</t>
+  </si>
+  <si>
+    <t>Exports your currently equipped gear, inventory, or all the items in your current Lua files' sets into gearswap .lua or spellcast .xml format. Takes options "inventory", "sets", and "xml." Defaults to currently equipped gear and lua otherwise.</t>
   </si>
 </sst>
 </file>
@@ -917,14 +917,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,21 +1229,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="D124" workbookViewId="0">
+      <selection activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="124.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="124.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="25.9" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:7" ht="25.95" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1256,17 +1256,17 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
@@ -1279,8 +1279,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1291,8 +1291,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1303,8 +1303,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1315,8 +1315,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="10"/>
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -1327,8 +1327,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="10"/>
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -1339,8 +1339,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -1351,8 +1351,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
       <c r="C11" t="s">
         <v>16</v>
       </c>
@@ -1363,8 +1363,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -1375,8 +1375,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
       <c r="C13" t="s">
         <v>20</v>
       </c>
@@ -1387,8 +1387,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
       <c r="C14" t="s">
         <v>77</v>
       </c>
@@ -1399,8 +1399,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="10"/>
       <c r="C15" t="s">
         <v>79</v>
       </c>
@@ -1411,8 +1411,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
       <c r="C16" t="s">
         <v>81</v>
       </c>
@@ -1423,8 +1423,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="10"/>
       <c r="C17" t="s">
         <v>83</v>
       </c>
@@ -1435,8 +1435,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
       <c r="C18" t="s">
         <v>85</v>
       </c>
@@ -1447,8 +1447,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="10"/>
       <c r="C19" t="s">
         <v>87</v>
       </c>
@@ -1459,8 +1459,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
@@ -1473,8 +1473,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="10"/>
       <c r="C23" t="s">
         <v>26</v>
       </c>
@@ -1485,8 +1485,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
       <c r="C24" t="s">
         <v>31</v>
       </c>
@@ -1497,8 +1497,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
       <c r="C25" t="s">
         <v>33</v>
       </c>
@@ -1509,8 +1509,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="10"/>
       <c r="C26" t="s">
         <v>35</v>
       </c>
@@ -1521,8 +1521,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
       <c r="C27" t="s">
         <v>37</v>
       </c>
@@ -1533,8 +1533,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
       <c r="C28" t="s">
         <v>38</v>
       </c>
@@ -1545,8 +1545,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="10"/>
       <c r="C29" t="s">
         <v>41</v>
       </c>
@@ -1557,8 +1557,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
       <c r="C30" t="s">
         <v>43</v>
       </c>
@@ -1569,8 +1569,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="10"/>
       <c r="C31" t="s">
         <v>45</v>
       </c>
@@ -1581,8 +1581,8 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="10"/>
       <c r="C32" t="s">
         <v>46</v>
       </c>
@@ -1593,8 +1593,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="10"/>
       <c r="C33" t="s">
         <v>47</v>
       </c>
@@ -1605,8 +1605,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="10"/>
       <c r="C34" t="s">
         <v>48</v>
       </c>
@@ -1617,8 +1617,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="10"/>
       <c r="C35" t="s">
         <v>54</v>
       </c>
@@ -1629,8 +1629,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="10"/>
       <c r="C36" t="s">
         <v>56</v>
       </c>
@@ -1641,8 +1641,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
       <c r="C37" t="s">
         <v>72</v>
       </c>
@@ -1653,8 +1653,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="10"/>
       <c r="C38" t="s">
         <v>73</v>
       </c>
@@ -1665,8 +1665,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="10"/>
       <c r="C39" t="s">
         <v>74</v>
       </c>
@@ -1677,8 +1677,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="10"/>
       <c r="C40" t="s">
         <v>75</v>
       </c>
@@ -1689,8 +1689,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="10"/>
       <c r="C41" t="s">
         <v>76</v>
       </c>
@@ -1701,8 +1701,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="8"/>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
       <c r="E42" t="s">
         <v>94</v>
       </c>
@@ -1710,8 +1710,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="10"/>
       <c r="E43" t="s">
         <v>95</v>
       </c>
@@ -1719,8 +1719,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="10"/>
       <c r="C44" t="s">
         <v>2</v>
       </c>
@@ -1731,8 +1731,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="10"/>
       <c r="E45" t="s">
         <v>97</v>
       </c>
@@ -1740,8 +1740,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
       <c r="E46" t="s">
         <v>98</v>
       </c>
@@ -1749,8 +1749,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="8"/>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="10"/>
       <c r="C47" t="s">
         <v>99</v>
       </c>
@@ -1761,8 +1761,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="8"/>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="10"/>
       <c r="C48" t="s">
         <v>100</v>
       </c>
@@ -1773,8 +1773,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="8"/>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
       <c r="C49" t="s">
         <v>101</v>
       </c>
@@ -1785,8 +1785,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="10"/>
       <c r="C50" t="s">
         <v>102</v>
       </c>
@@ -1797,14 +1797,14 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="8"/>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="10"/>
       <c r="C51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="8" t="s">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="10" t="s">
         <v>104</v>
       </c>
       <c r="C55" t="s">
@@ -1817,8 +1817,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="8"/>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="10"/>
       <c r="C56" t="s">
         <v>107</v>
       </c>
@@ -1829,8 +1829,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="8"/>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="10"/>
       <c r="C57" t="s">
         <v>109</v>
       </c>
@@ -1841,8 +1841,8 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="8"/>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="10"/>
       <c r="C58" t="s">
         <v>111</v>
       </c>
@@ -1853,8 +1853,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="8"/>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="10"/>
       <c r="C59" t="s">
         <v>115</v>
       </c>
@@ -1865,8 +1865,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="8"/>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="10"/>
       <c r="C60" t="s">
         <v>113</v>
       </c>
@@ -1877,8 +1877,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="8" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="10" t="s">
         <v>116</v>
       </c>
       <c r="C63" t="s">
@@ -1891,8 +1891,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="8"/>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="10"/>
       <c r="C64" t="s">
         <v>118</v>
       </c>
@@ -1903,8 +1903,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="8"/>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="10"/>
       <c r="C65" t="s">
         <v>119</v>
       </c>
@@ -1915,8 +1915,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="8" t="s">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C68" t="s">
@@ -1929,8 +1929,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="8"/>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="10"/>
       <c r="C69" t="s">
         <v>58</v>
       </c>
@@ -1941,8 +1941,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="8"/>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B70" s="10"/>
       <c r="C70" t="s">
         <v>60</v>
       </c>
@@ -1953,8 +1953,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="8"/>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="10"/>
       <c r="C71" t="s">
         <v>63</v>
       </c>
@@ -1965,8 +1965,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="8"/>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72" s="10"/>
       <c r="C72" t="s">
         <v>64</v>
       </c>
@@ -1977,8 +1977,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="8"/>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73" s="10"/>
       <c r="C73" t="s">
         <v>66</v>
       </c>
@@ -1989,8 +1989,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="8"/>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74" s="10"/>
       <c r="C74" t="s">
         <v>68</v>
       </c>
@@ -2001,8 +2001,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="8"/>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75" s="10"/>
       <c r="C75" t="s">
         <v>69</v>
       </c>
@@ -2013,8 +2013,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="8" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B78" s="10" t="s">
         <v>178</v>
       </c>
       <c r="C78" t="s">
@@ -2027,8 +2027,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="8"/>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="10"/>
       <c r="C79" t="s">
         <v>2</v>
       </c>
@@ -2039,8 +2039,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="8"/>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B80" s="10"/>
       <c r="C80" t="s">
         <v>2</v>
       </c>
@@ -2051,8 +2051,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="8"/>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81" s="10"/>
       <c r="C81" t="s">
         <v>2</v>
       </c>
@@ -2077,8 +2077,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="86" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="8" t="s">
+    <row r="86" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="10" t="s">
         <v>127</v>
       </c>
       <c r="C86" t="s">
@@ -2091,8 +2091,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="8"/>
+    <row r="87" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="10"/>
       <c r="C87" t="s">
         <v>132</v>
       </c>
@@ -2103,23 +2103,23 @@
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="8"/>
+    <row r="88" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="10"/>
       <c r="C88" t="s">
         <v>139</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E88" t="s">
         <v>262</v>
       </c>
-      <c r="E88" t="s">
+      <c r="G88" t="s">
         <v>263</v>
       </c>
-      <c r="G88" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="8"/>
+    </row>
+    <row r="89" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="10"/>
       <c r="C89" t="s">
         <v>140</v>
       </c>
@@ -2130,8 +2130,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="8"/>
+    <row r="90" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="10"/>
       <c r="C90" t="s">
         <v>125</v>
       </c>
@@ -2142,8 +2142,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="91" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="8"/>
+    <row r="91" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="10"/>
       <c r="C91" t="s">
         <v>149</v>
       </c>
@@ -2154,8 +2154,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="8"/>
+    <row r="92" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="10"/>
       <c r="C92" t="s">
         <v>2</v>
       </c>
@@ -2166,8 +2166,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="8"/>
+    <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="10"/>
       <c r="C93" t="s">
         <v>2</v>
       </c>
@@ -2178,8 +2178,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="8"/>
+    <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="10"/>
       <c r="C94" t="s">
         <v>2</v>
       </c>
@@ -2190,8 +2190,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="8"/>
+    <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="10"/>
       <c r="C95" t="s">
         <v>2</v>
       </c>
@@ -2202,8 +2202,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="8"/>
+    <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="10"/>
       <c r="C96" t="s">
         <v>2</v>
       </c>
@@ -2214,8 +2214,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="8"/>
+    <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="10"/>
       <c r="C97" t="s">
         <v>2</v>
       </c>
@@ -2226,8 +2226,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="8"/>
+    <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="10"/>
       <c r="C98" t="s">
         <v>2</v>
       </c>
@@ -2238,8 +2238,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="8"/>
+    <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="10"/>
       <c r="C99" t="s">
         <v>243</v>
       </c>
@@ -2250,8 +2250,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="8"/>
+    <row r="100" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="10"/>
       <c r="C100" t="s">
         <v>130</v>
       </c>
@@ -2262,8 +2262,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="8"/>
+    <row r="101" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="10"/>
       <c r="C101" t="s">
         <v>133</v>
       </c>
@@ -2274,8 +2274,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="8"/>
+    <row r="102" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="10"/>
       <c r="C102" t="s">
         <v>134</v>
       </c>
@@ -2286,11 +2286,11 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="10" t="s">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B104" s="9" t="s">
         <v>220</v>
       </c>
       <c r="E104" t="s">
@@ -2300,8 +2300,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="10"/>
+    <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="9"/>
       <c r="C105" t="s">
         <v>211</v>
       </c>
@@ -2312,8 +2312,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="10"/>
+    <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="9"/>
       <c r="C106" t="s">
         <v>212</v>
       </c>
@@ -2324,8 +2324,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="10"/>
+    <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="9"/>
       <c r="C107" t="s">
         <v>213</v>
       </c>
@@ -2336,8 +2336,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="10"/>
+    <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="9"/>
       <c r="E108" t="s">
         <v>216</v>
       </c>
@@ -2345,8 +2345,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="10"/>
+    <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="9"/>
       <c r="E109" t="s">
         <v>215</v>
       </c>
@@ -2354,8 +2354,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="10"/>
+    <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="9"/>
       <c r="E110" t="s">
         <v>237</v>
       </c>
@@ -2363,8 +2363,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="10"/>
+    <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="9"/>
       <c r="E111" t="s">
         <v>214</v>
       </c>
@@ -2372,8 +2372,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="10"/>
+    <row r="112" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="9"/>
       <c r="E112" t="s">
         <v>221</v>
       </c>
@@ -2381,8 +2381,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="10"/>
+    <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="9"/>
       <c r="E113" t="s">
         <v>239</v>
       </c>
@@ -2390,8 +2390,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="116" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="8" t="s">
+    <row r="116" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="10" t="s">
         <v>136</v>
       </c>
       <c r="C116" t="s">
@@ -2404,8 +2404,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="117" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="8"/>
+    <row r="117" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B117" s="10"/>
       <c r="C117" t="s">
         <v>124</v>
       </c>
@@ -2416,8 +2416,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="118" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="8"/>
+    <row r="118" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="10"/>
       <c r="C118" t="s">
         <v>126</v>
       </c>
@@ -2428,8 +2428,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="8"/>
+    <row r="119" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="10"/>
       <c r="C119" t="s">
         <v>133</v>
       </c>
@@ -2440,8 +2440,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="8"/>
+    <row r="120" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="10"/>
       <c r="C120" t="s">
         <v>134</v>
       </c>
@@ -2452,8 +2452,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="121" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="8"/>
+    <row r="121" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="10"/>
       <c r="C121" t="s">
         <v>137</v>
       </c>
@@ -2464,8 +2464,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="8"/>
+    <row r="122" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="10"/>
       <c r="C122" t="s">
         <v>130</v>
       </c>
@@ -2476,11 +2476,11 @@
         <v>247</v>
       </c>
     </row>
-    <row r="123" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="3"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="10" t="s">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B125" s="9" t="s">
         <v>154</v>
       </c>
       <c r="C125" t="s">
@@ -2493,8 +2493,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126" s="10"/>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B126" s="9"/>
       <c r="C126" t="s">
         <v>2</v>
       </c>
@@ -2505,8 +2505,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="10"/>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B127" s="9"/>
       <c r="C127" t="s">
         <v>2</v>
       </c>
@@ -2517,8 +2517,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B128" s="10"/>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B128" s="9"/>
       <c r="C128" t="s">
         <v>2</v>
       </c>
@@ -2529,8 +2529,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B129" s="10"/>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B129" s="9"/>
       <c r="C129" t="s">
         <v>2</v>
       </c>
@@ -2541,8 +2541,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B130" s="10"/>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B130" s="9"/>
       <c r="C130" t="s">
         <v>2</v>
       </c>
@@ -2553,8 +2553,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B131" s="10"/>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B131" s="9"/>
       <c r="C131" t="s">
         <v>2</v>
       </c>
@@ -2565,8 +2565,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B132" s="10"/>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B132" s="9"/>
       <c r="C132" t="s">
         <v>2</v>
       </c>
@@ -2577,8 +2577,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="8" t="s">
+    <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="10" t="s">
         <v>225</v>
       </c>
       <c r="E135" t="s">
@@ -2588,8 +2588,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="8"/>
+    <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="10"/>
       <c r="E136" t="s">
         <v>228</v>
       </c>
@@ -2597,8 +2597,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="137" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="8"/>
+    <row r="137" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="10"/>
       <c r="E137" t="s">
         <v>230</v>
       </c>
@@ -2606,8 +2606,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="8"/>
+    <row r="138" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="10"/>
       <c r="E138" t="s">
         <v>231</v>
       </c>
@@ -2615,8 +2615,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="139" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="8"/>
+    <row r="139" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="10"/>
       <c r="E139" t="s">
         <v>235</v>
       </c>
@@ -2624,8 +2624,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="8"/>
+    <row r="140" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B140" s="10"/>
       <c r="C140" t="s">
         <v>259</v>
       </c>
@@ -2633,29 +2633,30 @@
         <v>260</v>
       </c>
       <c r="G140" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="8"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="10"/>
       <c r="E141" t="s">
+        <v>265</v>
+      </c>
+      <c r="G141" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B142" s="10"/>
+      <c r="E142" t="s">
+        <v>264</v>
+      </c>
+      <c r="G142" t="s">
         <v>266</v>
-      </c>
-      <c r="G141" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B142" s="8"/>
-      <c r="E142" t="s">
-        <v>265</v>
-      </c>
-      <c r="G142" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B135:B142"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="B125:B132"/>
     <mergeCell ref="B78:B81"/>
@@ -2667,7 +2668,6 @@
     <mergeCell ref="B68:B75"/>
     <mergeCell ref="B104:B113"/>
     <mergeCell ref="B86:B102"/>
-    <mergeCell ref="B135:B142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2680,7 +2680,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2692,7 +2692,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Gearswap v0.708 - Encumbrance Support (and friends)
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -832,10 +832,10 @@
     <t>Disables equip commands targeting a given slot. "All" will prevent all equip commands. Providing no second argument will disable user gearswap file execution, although registered events will still run.</t>
   </si>
   <si>
-    <t>Enables equip commands targeting a given slot. "All" will allow all equip commands. Providing no second argument will enable user gearswap file execution, although registered events will still run.</t>
-  </si>
-  <si>
     <t>Exports your currently equipped gear, inventory, or all the items in your current Lua files' sets into gearswap .lua or spellcast .xml format. Takes options "inventory", "sets", and "xml." Defaults to currently equipped gear and lua otherwise.</t>
+  </si>
+  <si>
+    <t>Enables equip commands targeting a given slot. "All" will allow all equip commands. Providing no second argument will enable user gearswap file execution, if it was disabled.</t>
   </si>
 </sst>
 </file>
@@ -917,14 +917,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,21 +1229,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D124" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView tabSelected="1" topLeftCell="G124" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="124.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="124.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="25.95" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:7" ht="25.9" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1256,17 +1256,17 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C2" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
@@ -1279,8 +1279,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1291,8 +1291,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="10"/>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1303,8 +1303,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1315,8 +1315,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="10"/>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -1327,8 +1327,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="10"/>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -1339,8 +1339,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -1351,8 +1351,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
       <c r="C11" t="s">
         <v>16</v>
       </c>
@@ -1363,8 +1363,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -1375,8 +1375,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>20</v>
       </c>
@@ -1387,8 +1387,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
       <c r="C14" t="s">
         <v>77</v>
       </c>
@@ -1399,8 +1399,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
       <c r="C15" t="s">
         <v>79</v>
       </c>
@@ -1411,8 +1411,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
       <c r="C16" t="s">
         <v>81</v>
       </c>
@@ -1423,8 +1423,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>83</v>
       </c>
@@ -1435,8 +1435,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>85</v>
       </c>
@@ -1447,8 +1447,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
       <c r="C19" t="s">
         <v>87</v>
       </c>
@@ -1459,8 +1459,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
@@ -1473,8 +1473,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
       <c r="C23" t="s">
         <v>26</v>
       </c>
@@ -1485,8 +1485,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
       <c r="C24" t="s">
         <v>31</v>
       </c>
@@ -1497,8 +1497,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
       <c r="C25" t="s">
         <v>33</v>
       </c>
@@ -1509,8 +1509,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
       <c r="C26" t="s">
         <v>35</v>
       </c>
@@ -1521,8 +1521,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
       <c r="C27" t="s">
         <v>37</v>
       </c>
@@ -1533,8 +1533,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
       <c r="C28" t="s">
         <v>38</v>
       </c>
@@ -1545,8 +1545,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
       <c r="C29" t="s">
         <v>41</v>
       </c>
@@ -1557,8 +1557,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
       <c r="C30" t="s">
         <v>43</v>
       </c>
@@ -1569,8 +1569,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="10"/>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
       <c r="C31" t="s">
         <v>45</v>
       </c>
@@ -1581,8 +1581,8 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
       <c r="C32" t="s">
         <v>46</v>
       </c>
@@ -1593,8 +1593,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="10"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
       <c r="C33" t="s">
         <v>47</v>
       </c>
@@ -1605,8 +1605,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="10"/>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
       <c r="C34" t="s">
         <v>48</v>
       </c>
@@ -1617,8 +1617,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="10"/>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
       <c r="C35" t="s">
         <v>54</v>
       </c>
@@ -1629,8 +1629,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="10"/>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
       <c r="C36" t="s">
         <v>56</v>
       </c>
@@ -1641,8 +1641,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="10"/>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
       <c r="C37" t="s">
         <v>72</v>
       </c>
@@ -1653,8 +1653,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="10"/>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
       <c r="C38" t="s">
         <v>73</v>
       </c>
@@ -1665,8 +1665,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="10"/>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
       <c r="C39" t="s">
         <v>74</v>
       </c>
@@ -1677,8 +1677,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="10"/>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="8"/>
       <c r="C40" t="s">
         <v>75</v>
       </c>
@@ -1689,8 +1689,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="10"/>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="8"/>
       <c r="C41" t="s">
         <v>76</v>
       </c>
@@ -1701,8 +1701,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="10"/>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="8"/>
       <c r="E42" t="s">
         <v>94</v>
       </c>
@@ -1710,8 +1710,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="10"/>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="8"/>
       <c r="E43" t="s">
         <v>95</v>
       </c>
@@ -1719,8 +1719,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="10"/>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="8"/>
       <c r="C44" t="s">
         <v>2</v>
       </c>
@@ -1731,8 +1731,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="10"/>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="8"/>
       <c r="E45" t="s">
         <v>97</v>
       </c>
@@ -1740,8 +1740,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="10"/>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="8"/>
       <c r="E46" t="s">
         <v>98</v>
       </c>
@@ -1749,8 +1749,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="10"/>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
       <c r="C47" t="s">
         <v>99</v>
       </c>
@@ -1761,8 +1761,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="10"/>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="8"/>
       <c r="C48" t="s">
         <v>100</v>
       </c>
@@ -1773,8 +1773,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="10"/>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="8"/>
       <c r="C49" t="s">
         <v>101</v>
       </c>
@@ -1785,8 +1785,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="10"/>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="8"/>
       <c r="C50" t="s">
         <v>102</v>
       </c>
@@ -1797,14 +1797,14 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="10"/>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="8"/>
       <c r="C51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="10" t="s">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C55" t="s">
@@ -1817,8 +1817,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="10"/>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="8"/>
       <c r="C56" t="s">
         <v>107</v>
       </c>
@@ -1829,8 +1829,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="10"/>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
       <c r="C57" t="s">
         <v>109</v>
       </c>
@@ -1841,8 +1841,8 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="10"/>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="8"/>
       <c r="C58" t="s">
         <v>111</v>
       </c>
@@ -1853,8 +1853,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="10"/>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
       <c r="C59" t="s">
         <v>115</v>
       </c>
@@ -1865,8 +1865,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="10"/>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="8"/>
       <c r="C60" t="s">
         <v>113</v>
       </c>
@@ -1877,8 +1877,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="10" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
         <v>116</v>
       </c>
       <c r="C63" t="s">
@@ -1891,8 +1891,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="10"/>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="8"/>
       <c r="C64" t="s">
         <v>118</v>
       </c>
@@ -1903,8 +1903,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B65" s="10"/>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="8"/>
       <c r="C65" t="s">
         <v>119</v>
       </c>
@@ -1915,8 +1915,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="10" t="s">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C68" t="s">
@@ -1929,8 +1929,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B69" s="10"/>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="8"/>
       <c r="C69" t="s">
         <v>58</v>
       </c>
@@ -1941,8 +1941,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B70" s="10"/>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="8"/>
       <c r="C70" t="s">
         <v>60</v>
       </c>
@@ -1953,8 +1953,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B71" s="10"/>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
       <c r="C71" t="s">
         <v>63</v>
       </c>
@@ -1965,8 +1965,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" s="10"/>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
       <c r="C72" t="s">
         <v>64</v>
       </c>
@@ -1977,8 +1977,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B73" s="10"/>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
       <c r="C73" t="s">
         <v>66</v>
       </c>
@@ -1989,8 +1989,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B74" s="10"/>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
       <c r="C74" t="s">
         <v>68</v>
       </c>
@@ -2001,8 +2001,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B75" s="10"/>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="8"/>
       <c r="C75" t="s">
         <v>69</v>
       </c>
@@ -2013,8 +2013,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B78" s="10" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="8" t="s">
         <v>178</v>
       </c>
       <c r="C78" t="s">
@@ -2027,8 +2027,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B79" s="10"/>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="8"/>
       <c r="C79" t="s">
         <v>2</v>
       </c>
@@ -2039,8 +2039,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B80" s="10"/>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="8"/>
       <c r="C80" t="s">
         <v>2</v>
       </c>
@@ -2051,8 +2051,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B81" s="10"/>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="8"/>
       <c r="C81" t="s">
         <v>2</v>
       </c>
@@ -2077,8 +2077,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="86" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="10" t="s">
+    <row r="86" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C86" t="s">
@@ -2091,8 +2091,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="10"/>
+    <row r="87" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="8"/>
       <c r="C87" t="s">
         <v>132</v>
       </c>
@@ -2103,8 +2103,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="10"/>
+    <row r="88" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
       <c r="C88" t="s">
         <v>139</v>
       </c>
@@ -2118,8 +2118,8 @@
         <v>263</v>
       </c>
     </row>
-    <row r="89" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="10"/>
+    <row r="89" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="8"/>
       <c r="C89" t="s">
         <v>140</v>
       </c>
@@ -2130,8 +2130,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="10"/>
+    <row r="90" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="8"/>
       <c r="C90" t="s">
         <v>125</v>
       </c>
@@ -2142,8 +2142,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="91" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="10"/>
+    <row r="91" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
       <c r="C91" t="s">
         <v>149</v>
       </c>
@@ -2154,8 +2154,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="10"/>
+    <row r="92" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
       <c r="C92" t="s">
         <v>2</v>
       </c>
@@ -2166,8 +2166,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="10"/>
+    <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="8"/>
       <c r="C93" t="s">
         <v>2</v>
       </c>
@@ -2178,8 +2178,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="10"/>
+    <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
       <c r="C94" t="s">
         <v>2</v>
       </c>
@@ -2190,8 +2190,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="10"/>
+    <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="8"/>
       <c r="C95" t="s">
         <v>2</v>
       </c>
@@ -2202,8 +2202,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="10"/>
+    <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="8"/>
       <c r="C96" t="s">
         <v>2</v>
       </c>
@@ -2214,8 +2214,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="10"/>
+    <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="8"/>
       <c r="C97" t="s">
         <v>2</v>
       </c>
@@ -2226,8 +2226,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="10"/>
+    <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="8"/>
       <c r="C98" t="s">
         <v>2</v>
       </c>
@@ -2238,8 +2238,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="10"/>
+    <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="8"/>
       <c r="C99" t="s">
         <v>243</v>
       </c>
@@ -2250,8 +2250,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="10"/>
+    <row r="100" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="8"/>
       <c r="C100" t="s">
         <v>130</v>
       </c>
@@ -2262,8 +2262,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="10"/>
+    <row r="101" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="8"/>
       <c r="C101" t="s">
         <v>133</v>
       </c>
@@ -2274,8 +2274,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="10"/>
+    <row r="102" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
       <c r="C102" t="s">
         <v>134</v>
       </c>
@@ -2286,11 +2286,11 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B104" s="9" t="s">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="10" t="s">
         <v>220</v>
       </c>
       <c r="E104" t="s">
@@ -2300,8 +2300,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="9"/>
+    <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="10"/>
       <c r="C105" t="s">
         <v>211</v>
       </c>
@@ -2312,8 +2312,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="9"/>
+    <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="10"/>
       <c r="C106" t="s">
         <v>212</v>
       </c>
@@ -2324,8 +2324,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="9"/>
+    <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="10"/>
       <c r="C107" t="s">
         <v>213</v>
       </c>
@@ -2336,8 +2336,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="9"/>
+    <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="10"/>
       <c r="E108" t="s">
         <v>216</v>
       </c>
@@ -2345,8 +2345,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="9"/>
+    <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="10"/>
       <c r="E109" t="s">
         <v>215</v>
       </c>
@@ -2354,8 +2354,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="9"/>
+    <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="10"/>
       <c r="E110" t="s">
         <v>237</v>
       </c>
@@ -2363,8 +2363,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="9"/>
+    <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="10"/>
       <c r="E111" t="s">
         <v>214</v>
       </c>
@@ -2372,8 +2372,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="9"/>
+    <row r="112" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="10"/>
       <c r="E112" t="s">
         <v>221</v>
       </c>
@@ -2381,8 +2381,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="9"/>
+    <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="10"/>
       <c r="E113" t="s">
         <v>239</v>
       </c>
@@ -2390,8 +2390,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="116" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="10" t="s">
+    <row r="116" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C116" t="s">
@@ -2404,8 +2404,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="117" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="10"/>
+    <row r="117" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="8"/>
       <c r="C117" t="s">
         <v>124</v>
       </c>
@@ -2416,8 +2416,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="118" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="10"/>
+    <row r="118" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="8"/>
       <c r="C118" t="s">
         <v>126</v>
       </c>
@@ -2428,8 +2428,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="10"/>
+    <row r="119" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="8"/>
       <c r="C119" t="s">
         <v>133</v>
       </c>
@@ -2440,8 +2440,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="10"/>
+    <row r="120" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="8"/>
       <c r="C120" t="s">
         <v>134</v>
       </c>
@@ -2452,8 +2452,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="121" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="10"/>
+    <row r="121" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="8"/>
       <c r="C121" t="s">
         <v>137</v>
       </c>
@@ -2464,8 +2464,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="10"/>
+    <row r="122" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="8"/>
       <c r="C122" t="s">
         <v>130</v>
       </c>
@@ -2476,11 +2476,11 @@
         <v>247</v>
       </c>
     </row>
-    <row r="123" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="3"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B125" s="9" t="s">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="10" t="s">
         <v>154</v>
       </c>
       <c r="C125" t="s">
@@ -2493,8 +2493,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B126" s="9"/>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="10"/>
       <c r="C126" t="s">
         <v>2</v>
       </c>
@@ -2505,8 +2505,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B127" s="9"/>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="10"/>
       <c r="C127" t="s">
         <v>2</v>
       </c>
@@ -2517,8 +2517,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B128" s="9"/>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="10"/>
       <c r="C128" t="s">
         <v>2</v>
       </c>
@@ -2529,8 +2529,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B129" s="9"/>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B129" s="10"/>
       <c r="C129" t="s">
         <v>2</v>
       </c>
@@ -2541,8 +2541,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B130" s="9"/>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="10"/>
       <c r="C130" t="s">
         <v>2</v>
       </c>
@@ -2553,8 +2553,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B131" s="9"/>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="10"/>
       <c r="C131" t="s">
         <v>2</v>
       </c>
@@ -2565,8 +2565,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B132" s="9"/>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="10"/>
       <c r="C132" t="s">
         <v>2</v>
       </c>
@@ -2577,8 +2577,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="10" t="s">
+    <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="8" t="s">
         <v>225</v>
       </c>
       <c r="E135" t="s">
@@ -2588,8 +2588,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="10"/>
+    <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="8"/>
       <c r="E136" t="s">
         <v>228</v>
       </c>
@@ -2597,8 +2597,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="137" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="10"/>
+    <row r="137" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="8"/>
       <c r="E137" t="s">
         <v>230</v>
       </c>
@@ -2606,8 +2606,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="10"/>
+    <row r="138" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="8"/>
       <c r="E138" t="s">
         <v>231</v>
       </c>
@@ -2615,8 +2615,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="139" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="10"/>
+    <row r="139" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="8"/>
       <c r="E139" t="s">
         <v>235</v>
       </c>
@@ -2624,8 +2624,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="10"/>
+    <row r="140" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="8"/>
       <c r="C140" t="s">
         <v>259</v>
       </c>
@@ -2633,20 +2633,20 @@
         <v>260</v>
       </c>
       <c r="G140" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="10"/>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="8"/>
       <c r="E141" t="s">
         <v>265</v>
       </c>
       <c r="G141" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B142" s="10"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="8"/>
       <c r="E142" t="s">
         <v>264</v>
       </c>
@@ -2680,7 +2680,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2692,7 +2692,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Gearswap - Minor documentation update
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variable Remapping.xlsx
@@ -513,9 +513,6 @@
     <t>Whatever was entered as a target.</t>
   </si>
   <si>
-    <t>Table of Booleans keyed to 'Self', 'Player', 'Party', 'Ally', 'NPC', and 'Enemy'. True means that it's valid for that target.</t>
-  </si>
-  <si>
     <t>Pulled from the player array.</t>
   </si>
   <si>
@@ -839,6 +836,9 @@
   </si>
   <si>
     <t>SELF', 'PLAYER', 'NPC', or 'MONSTER'. Should be re-keyed to match validtarget.</t>
+  </si>
+  <si>
+    <t>Table of Booleans keyed to 'Self', 'Player', 'Party', 'Ally', 'NPC', 'Enemy', and 'Corpse'. True means that it's valid for that target.</t>
   </si>
 </sst>
 </file>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1303,7 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>165</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
         <v>82</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>84</v>
       </c>
       <c r="G17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>86</v>
       </c>
       <c r="G18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
         <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
         <v>34</v>
       </c>
       <c r="G25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1521,7 +1521,7 @@
         <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1533,7 +1533,7 @@
         <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1545,7 +1545,7 @@
         <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>49</v>
       </c>
       <c r="G31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1593,7 +1593,7 @@
         <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -1617,7 +1617,7 @@
         <v>52</v>
       </c>
       <c r="G34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
         <v>55</v>
       </c>
       <c r="G35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
         <v>57</v>
       </c>
       <c r="G36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>89</v>
       </c>
       <c r="G37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -1665,7 +1665,7 @@
         <v>90</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>91</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -1689,7 +1689,7 @@
         <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>93</v>
       </c>
       <c r="G41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>94</v>
       </c>
       <c r="G42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>95</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
@@ -1731,7 +1731,7 @@
         <v>96</v>
       </c>
       <c r="G44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>97</v>
       </c>
       <c r="G45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>98</v>
       </c>
       <c r="G46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
@@ -1761,7 +1761,7 @@
         <v>120</v>
       </c>
       <c r="G47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -1773,7 +1773,7 @@
         <v>121</v>
       </c>
       <c r="G48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -1785,7 +1785,7 @@
         <v>122</v>
       </c>
       <c r="G49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
@@ -1797,7 +1797,7 @@
         <v>123</v>
       </c>
       <c r="G50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
         <v>106</v>
       </c>
       <c r="G55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1829,7 +1829,7 @@
         <v>108</v>
       </c>
       <c r="G56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
         <v>110</v>
       </c>
       <c r="G57" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,7 @@
         <v>112</v>
       </c>
       <c r="G58" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
         <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
@@ -1903,7 +1903,7 @@
         <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>30</v>
       </c>
       <c r="G68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -1941,7 +1941,7 @@
         <v>59</v>
       </c>
       <c r="G69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
@@ -1953,7 +1953,7 @@
         <v>61</v>
       </c>
       <c r="G70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
@@ -1965,7 +1965,7 @@
         <v>62</v>
       </c>
       <c r="G71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>65</v>
       </c>
       <c r="G72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>67</v>
       </c>
       <c r="G73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
@@ -2001,7 +2001,7 @@
         <v>70</v>
       </c>
       <c r="G74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
@@ -2013,21 +2013,21 @@
         <v>71</v>
       </c>
       <c r="G75" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C78" t="s">
         <v>53</v>
       </c>
       <c r="E78" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
@@ -2036,10 +2036,10 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
+        <v>178</v>
+      </c>
+      <c r="G79" t="s">
         <v>179</v>
-      </c>
-      <c r="G79" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
@@ -2048,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -2060,10 +2060,10 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="2:7" ht="21" x14ac:dyDescent="0.35">
@@ -2077,7 +2077,7 @@
         <v>129</v>
       </c>
       <c r="G83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
         <v>144</v>
       </c>
       <c r="G86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2100,10 +2100,10 @@
         <v>132</v>
       </c>
       <c r="E87" t="s">
+        <v>186</v>
+      </c>
+      <c r="G87" t="s">
         <v>187</v>
-      </c>
-      <c r="G87" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="88" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2112,13 +2112,13 @@
         <v>139</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E88" t="s">
         <v>261</v>
       </c>
-      <c r="E88" t="s">
+      <c r="G88" t="s">
         <v>262</v>
-      </c>
-      <c r="G88" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="89" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2130,7 +2130,7 @@
         <v>142</v>
       </c>
       <c r="G89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2139,10 +2139,10 @@
         <v>125</v>
       </c>
       <c r="E90" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2151,10 +2151,10 @@
         <v>149</v>
       </c>
       <c r="E91" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G91" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
         <v>138</v>
       </c>
       <c r="G92" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="93" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,7 +2178,7 @@
         <v>148</v>
       </c>
       <c r="G93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2190,7 +2190,7 @@
         <v>145</v>
       </c>
       <c r="G94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="95" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>146</v>
       </c>
       <c r="G95" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
         <v>147</v>
       </c>
       <c r="G96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2223,10 +2223,10 @@
         <v>2</v>
       </c>
       <c r="E97" t="s">
+        <v>255</v>
+      </c>
+      <c r="G97" t="s">
         <v>256</v>
-      </c>
-      <c r="G97" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="98" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2235,22 +2235,22 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G98" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="8"/>
       <c r="C99" t="s">
+        <v>242</v>
+      </c>
+      <c r="E99" t="s">
         <v>243</v>
       </c>
-      <c r="E99" t="s">
+      <c r="G99" t="s">
         <v>244</v>
-      </c>
-      <c r="G99" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="100" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>2</v>
       </c>
       <c r="G100" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2271,10 +2271,10 @@
         <v>133</v>
       </c>
       <c r="E101" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G101" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="102" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2283,114 +2283,114 @@
         <v>134</v>
       </c>
       <c r="E102" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G102" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="2"/>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E104" t="s">
+        <v>240</v>
+      </c>
+      <c r="G104" t="s">
         <v>241</v>
-      </c>
-      <c r="G104" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="105" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="10"/>
       <c r="C105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G105" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="10"/>
       <c r="C106" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G106" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="107" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="10"/>
       <c r="C107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="10"/>
       <c r="E108" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="10"/>
       <c r="E109" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G109" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="110" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="10"/>
       <c r="E110" t="s">
+        <v>236</v>
+      </c>
+      <c r="G110" t="s">
         <v>237</v>
-      </c>
-      <c r="G110" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="111" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="10"/>
       <c r="E111" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G111" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="10"/>
       <c r="E112" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G112" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="10"/>
       <c r="E113" t="s">
+        <v>238</v>
+      </c>
+      <c r="G113" t="s">
         <v>239</v>
-      </c>
-      <c r="G113" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="116" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
         <v>2</v>
       </c>
       <c r="G116" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="117" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>2</v>
       </c>
       <c r="G118" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="119" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="G119" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
         <v>2</v>
       </c>
       <c r="G120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2464,7 +2464,7 @@
         <v>2</v>
       </c>
       <c r="G121" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="122" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2476,10 +2476,10 @@
         <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="3"/>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>150</v>
       </c>
       <c r="G125" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
         <v>151</v>
       </c>
       <c r="G126" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>152</v>
       </c>
       <c r="G127" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>153</v>
       </c>
       <c r="G128" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>155</v>
       </c>
       <c r="G129" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
@@ -2553,7 +2553,7 @@
         <v>156</v>
       </c>
       <c r="G130" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>157</v>
       </c>
       <c r="G131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
@@ -2577,84 +2577,84 @@
         <v>158</v>
       </c>
       <c r="G132" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E135" t="s">
         <v>225</v>
       </c>
-      <c r="E135" t="s">
+      <c r="G135" t="s">
         <v>226</v>
-      </c>
-      <c r="G135" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
       <c r="E136" t="s">
+        <v>227</v>
+      </c>
+      <c r="G136" t="s">
         <v>228</v>
-      </c>
-      <c r="G136" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="137" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="8"/>
       <c r="E137" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G137" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="138" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="8"/>
       <c r="E138" t="s">
+        <v>230</v>
+      </c>
+      <c r="G138" t="s">
         <v>231</v>
-      </c>
-      <c r="G138" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="139" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="8"/>
       <c r="E139" t="s">
+        <v>234</v>
+      </c>
+      <c r="G139" t="s">
         <v>235</v>
-      </c>
-      <c r="G139" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="140" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="8"/>
       <c r="C140" t="s">
+        <v>258</v>
+      </c>
+      <c r="E140" t="s">
         <v>259</v>
       </c>
-      <c r="E140" t="s">
-        <v>260</v>
-      </c>
       <c r="G140" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="141" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="8"/>
       <c r="E141" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G141" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="8"/>
       <c r="E142" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G142" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>